<commit_message>
Avances Grales. en capa de sevicios. Faltan probar los CRUD.
</commit_message>
<xml_diff>
--- a/Requerimientos de catedra.xlsx
+++ b/Requerimientos de catedra.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juandiaz\Desktop\DentalCare\DentalCare\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2901D3C9-DB77-4A3B-8731-E7C7A96B35AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +26,64 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Observer</t>
+  </si>
+  <si>
+    <t>Facade</t>
+  </si>
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>unitofwork</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>A mediohacer</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>(Rol)</t>
+  </si>
+  <si>
+    <t>(Permiso)</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Permiso</t>
+  </si>
+  <si>
+    <t>Rol-Rol</t>
+  </si>
+  <si>
+    <t>Rol-Permiso</t>
+  </si>
+  <si>
+    <t>Usuario-Rol</t>
+  </si>
+  <si>
+    <t>Usuario-Permiso</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +401,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19415CCD-ED29-4BF6-BB9C-674C36BB9A12}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>